<commit_message>
Add =BitMexInstrumentsActive() as alias for =BitMexInstruments("Open")
</commit_message>
<xml_diff>
--- a/BitMexExample.xlsx
+++ b/BitMexExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Bid</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>XBTJ15</t>
+  </si>
+  <si>
+    <t>(ctrl-shift-enter to refresh)</t>
+  </si>
+  <si>
+    <t>(automatically updates)</t>
+  </si>
+  <si>
+    <t>level</t>
   </si>
 </sst>
 </file>
@@ -169,96 +178,102 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.7359b63b0a1c4d6fa3f7399526570ab5">
-      <tp>
-        <v>241.3</v>
+    <main first="rtdsrv.0e1baffb42944ede84f90876903fe9e0">
+      <tp>
+        <v>240</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Bid</stp>
+        <stp>4</stp>
+        <tr r="D9" s="1"/>
+      </tp>
+      <tp>
+        <v>241</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Bid</stp>
         <stp>3</stp>
-        <tr r="D7" s="1"/>
-      </tp>
-      <tp>
-        <v>241.74</v>
+        <tr r="D8" s="1"/>
+      </tp>
+      <tp>
+        <v>242.25</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Bid</stp>
         <stp>2</stp>
-        <tr r="D6" s="1"/>
-      </tp>
-      <tp>
-        <v>242.1</v>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp>
+        <v>243.27</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Bid</stp>
         <stp>1</stp>
-        <tr r="D5" s="1"/>
-      </tp>
-      <tp>
-        <v>242.46</v>
+        <tr r="D6" s="1"/>
+      </tp>
+      <tp>
+        <v>243.63</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Bid</stp>
         <stp>0</stp>
-        <tr r="D4" s="1"/>
-      </tp>
-      <tp>
-        <v>241</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Bid</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+      <tp>
+        <v>250</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Ask</stp>
         <stp>4</stp>
-        <tr r="D8" s="1"/>
-      </tp>
-      <tp>
-        <v>243.55</v>
+        <tr r="E9" s="1"/>
+      </tp>
+      <tp>
+        <v>244.95</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Ask</stp>
         <stp>0</stp>
-        <tr r="E4" s="1"/>
-      </tp>
-      <tp>
-        <v>243.8</v>
+        <tr r="E5" s="1"/>
+      </tp>
+      <tp>
+        <v>247.1</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Ask</stp>
         <stp>1</stp>
-        <tr r="E5" s="1"/>
-      </tp>
-      <tp>
-        <v>243.91</v>
+        <tr r="E6" s="1"/>
+      </tp>
+      <tp>
+        <v>247.64</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Ask</stp>
         <stp>2</stp>
-        <tr r="E6" s="1"/>
-      </tp>
-      <tp>
-        <v>244.28</v>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp>
+        <v>249.99</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Ask</stp>
         <stp>3</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp>
-        <v>247.59</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Ask</stp>
+        <tr r="E8" s="1"/>
+      </tp>
+      <tp>
+        <v>4601</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
         <stp>4</stp>
-        <tr r="E8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.7359b63b0a1c4d6fa3f7399526570ab5">
+        <tr r="C9" s="1"/>
+      </tp>
       <tp>
         <v>1000</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>BidVol</stp>
         <stp>1</stp>
-        <tr r="C5" s="1"/>
+        <tr r="C6" s="1"/>
       </tp>
       <tp>
         <v>1000</v>
@@ -266,7 +281,7 @@
         <stp>XBTJ15</stp>
         <stp>BidVol</stp>
         <stp>0</stp>
-        <tr r="C4" s="1"/>
+        <tr r="C5" s="1"/>
       </tp>
       <tp>
         <v>400</v>
@@ -274,33 +289,33 @@
         <stp>XBTJ15</stp>
         <stp>BidVol</stp>
         <stp>3</stp>
-        <tr r="C7" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
+        <tr r="C8" s="1"/>
+      </tp>
+      <tp>
+        <v>400</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>BidVol</stp>
         <stp>2</stp>
-        <tr r="C6" s="1"/>
-      </tp>
-      <tp>
-        <v>400</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.0e1baffb42944ede84f90876903fe9e0">
+      <tp>
+        <v>100</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>AskVol</stp>
         <stp>4</stp>
-        <tr r="C8" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.7359b63b0a1c4d6fa3f7399526570ab5">
+        <tr r="F9" s="1"/>
+      </tp>
       <tp>
         <v>400</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
         <stp>1</stp>
-        <tr r="F5" s="1"/>
+        <tr r="F6" s="1"/>
       </tp>
       <tp>
         <v>1000</v>
@@ -308,31 +323,23 @@
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
         <stp>0</stp>
-        <tr r="F4" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
+        <tr r="F5" s="1"/>
+      </tp>
+      <tp>
+        <v>300</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
         <stp>3</stp>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
+        <tr r="F8" s="1"/>
+      </tp>
+      <tp>
+        <v>133</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
         <stp>2</stp>
-        <tr r="F6" s="1"/>
-      </tp>
-      <tp>
-        <v>300</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>4</stp>
-        <tr r="F8" s="1"/>
+        <tr r="F7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -602,17 +609,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M18"/>
+  <dimension ref="A2:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -627,47 +634,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <f>_xll.BitMexBidVol($B$2, $B4)</f>
-        <v>1000</v>
-      </c>
-      <c r="D4" s="3">
-        <f>_xll.BitMexBid($B$2, $B4)</f>
-        <v>242.46</v>
-      </c>
-      <c r="E4" s="4">
-        <f>_xll.BitMexAsk($B$2, $B4)</f>
-        <v>243.55</v>
-      </c>
-      <c r="F4" s="4">
-        <f>_xll.BitMexAskVol($B$2, $B4)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
       </c>
       <c r="C5" s="3">
         <f>_xll.BitMexBidVol($B$2, $B5)</f>
@@ -675,20 +664,23 @@
       </c>
       <c r="D5" s="3">
         <f>_xll.BitMexBid($B$2, $B5)</f>
-        <v>242.1</v>
+        <v>243.63</v>
       </c>
       <c r="E5" s="4">
         <f>_xll.BitMexAsk($B$2, $B5)</f>
-        <v>243.8</v>
+        <v>244.95</v>
       </c>
       <c r="F5" s="4">
         <f>_xll.BitMexAskVol($B$2, $B5)</f>
-        <v>400</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <f>_xll.BitMexBidVol($B$2, $B6)</f>
@@ -696,20 +688,20 @@
       </c>
       <c r="D6" s="3">
         <f>_xll.BitMexBid($B$2, $B6)</f>
-        <v>241.74</v>
+        <v>243.27</v>
       </c>
       <c r="E6" s="4">
         <f>_xll.BitMexAsk($B$2, $B6)</f>
-        <v>243.91</v>
+        <v>247.1</v>
       </c>
       <c r="F6" s="4">
         <f>_xll.BitMexAskVol($B$2, $B6)</f>
-        <v>1000</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3">
         <f>_xll.BitMexBidVol($B$2, $B7)</f>
@@ -717,20 +709,20 @@
       </c>
       <c r="D7" s="3">
         <f>_xll.BitMexBid($B$2, $B7)</f>
-        <v>241.3</v>
+        <v>242.25</v>
       </c>
       <c r="E7" s="4">
         <f>_xll.BitMexAsk($B$2, $B7)</f>
-        <v>244.28</v>
+        <v>247.64</v>
       </c>
       <c r="F7" s="4">
         <f>_xll.BitMexAskVol($B$2, $B7)</f>
-        <v>1000</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <f>_xll.BitMexBidVol($B$2, $B8)</f>
@@ -742,7 +734,7 @@
       </c>
       <c r="E8" s="4">
         <f>_xll.BitMexAsk($B$2, $B8)</f>
-        <v>247.59</v>
+        <v>249.99</v>
       </c>
       <c r="F8" s="4">
         <f>_xll.BitMexAskVol($B$2, $B8)</f>
@@ -750,109 +742,95 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <f>_xll.BitMexBidVol($B$2, $B9)</f>
+        <v>4601</v>
+      </c>
+      <c r="D9" s="3">
+        <f>_xll.BitMexBid($B$2, $B9)</f>
+        <v>240</v>
+      </c>
+      <c r="E9" s="4">
+        <f>_xll.BitMexAsk($B$2, $B9)</f>
+        <v>250</v>
+      </c>
+      <c r="F9" s="4">
+        <f>_xll.BitMexAskVol($B$2, $B9)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="str">
-        <f t="array" ref="B11:M18">_xll.BitMexInstruments("Open")</f>
+      <c r="B12" s="5" t="str">
+        <f t="array" ref="B12:M19">_xll.BitMexInstrumentsActive()</f>
         <v>Symbol</v>
       </c>
-      <c r="C11" s="5" t="str">
+      <c r="C12" s="5" t="str">
         <v>RootSymbol</v>
       </c>
-      <c r="D11" s="5" t="str">
+      <c r="D12" s="5" t="str">
         <v>State</v>
       </c>
-      <c r="E11" s="5" t="str">
+      <c r="E12" s="5" t="str">
         <v>Typ</v>
       </c>
-      <c r="F11" s="5" t="str">
+      <c r="F12" s="5" t="str">
         <v>Expiry</v>
       </c>
-      <c r="G11" s="5" t="str">
+      <c r="G12" s="5" t="str">
         <v>TickSize</v>
       </c>
-      <c r="H11" s="5" t="str">
+      <c r="H12" s="5" t="str">
         <v>Multiplier</v>
       </c>
-      <c r="I11" s="5" t="str">
+      <c r="I12" s="5" t="str">
         <v>PrevClosePrice</v>
       </c>
-      <c r="J11" s="5" t="str">
+      <c r="J12" s="5" t="str">
         <v>TotalVolume</v>
       </c>
-      <c r="K11" s="5" t="str">
+      <c r="K12" s="5" t="str">
         <v>Volume</v>
       </c>
-      <c r="L11" s="5" t="str">
+      <c r="L12" s="5" t="str">
         <v>Vwap</v>
       </c>
-      <c r="M11" s="5" t="str">
+      <c r="M12" s="5" t="str">
         <v>OpenInterest</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" t="str">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="str">
         <v>BVOLJ15</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C13" t="str">
         <v>BVOL</v>
-      </c>
-      <c r="D12" t="str">
-        <v>Open</v>
-      </c>
-      <c r="E12" t="str">
-        <v>FFICSX</v>
-      </c>
-      <c r="F12" t="str">
-        <v>2015-04-24T12:00:00.000Z</v>
-      </c>
-      <c r="G12" t="str">
-        <v>0.01</v>
-      </c>
-      <c r="H12" t="str">
-        <v>1000000</v>
-      </c>
-      <c r="I12" t="str">
-        <v>60</v>
-      </c>
-      <c r="J12" t="str">
-        <v>0</v>
-      </c>
-      <c r="K12" t="str">
-        <v>0</v>
-      </c>
-      <c r="L12" t="str">
-        <v>0</v>
-      </c>
-      <c r="M12" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" t="str">
-        <v>XBTJ15</v>
-      </c>
-      <c r="C13" t="str">
-        <v>XBT</v>
       </c>
       <c r="D13" t="str">
         <v>Open</v>
       </c>
       <c r="E13" t="str">
-        <v>FXXXS</v>
+        <v>FFICSX</v>
       </c>
       <c r="F13" t="str">
         <v>2015-04-24T12:00:00.000Z</v>
@@ -861,30 +839,30 @@
         <v>0.01</v>
       </c>
       <c r="H13" t="str">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
       <c r="I13" t="str">
-        <v>246.02</v>
+        <v>60</v>
       </c>
       <c r="J13" t="str">
-        <v>195580</v>
+        <v>0</v>
       </c>
       <c r="K13" t="str">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L13" t="str">
-        <v>243.21</v>
+        <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>56467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
-        <v>XBUU15</v>
+        <v>XBTJ15</v>
       </c>
       <c r="C14" t="str">
-        <v>XBU</v>
+        <v>XBT</v>
       </c>
       <c r="D14" t="str">
         <v>Open</v>
@@ -893,33 +871,33 @@
         <v>FXXXS</v>
       </c>
       <c r="F14" t="str">
-        <v>2015-09-25T12:00:00.000Z</v>
+        <v>2015-04-24T12:00:00.000Z</v>
       </c>
       <c r="G14" t="str">
         <v>0.01</v>
       </c>
       <c r="H14" t="str">
-        <v>-10000000000</v>
+        <v>1000</v>
       </c>
       <c r="I14" t="str">
-        <v>244.28</v>
+        <v>246.02</v>
       </c>
       <c r="J14" t="str">
-        <v>5348</v>
+        <v>195581</v>
       </c>
       <c r="K14" t="str">
-        <v>0</v>
+        <v>1001</v>
       </c>
       <c r="L14" t="str">
-        <v>0</v>
+        <v>243.211</v>
       </c>
       <c r="M14" t="str">
-        <v>2215</v>
+        <v>56467</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
-        <v>XBUM15</v>
+        <v>XBUU15</v>
       </c>
       <c r="C15" t="str">
         <v>XBU</v>
@@ -931,7 +909,7 @@
         <v>FXXXS</v>
       </c>
       <c r="F15" t="str">
-        <v>2015-06-26T12:00:00.000Z</v>
+        <v>2015-09-25T12:00:00.000Z</v>
       </c>
       <c r="G15" t="str">
         <v>0.01</v>
@@ -940,24 +918,24 @@
         <v>-10000000000</v>
       </c>
       <c r="I15" t="str">
-        <v>248.49</v>
+        <v>244.28</v>
       </c>
       <c r="J15" t="str">
-        <v>3153</v>
+        <v>5349</v>
       </c>
       <c r="K15" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="str">
-        <v>0</v>
+        <v>242.12</v>
       </c>
       <c r="M15" t="str">
-        <v>1038</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
-        <v>XBUM15_U15</v>
+        <v>XBUM15</v>
       </c>
       <c r="C16" t="str">
         <v>XBU</v>
@@ -966,7 +944,7 @@
         <v>Open</v>
       </c>
       <c r="E16" t="str">
-        <v>FMXXS</v>
+        <v>FXXXS</v>
       </c>
       <c r="F16" t="str">
         <v>2015-06-26T12:00:00.000Z</v>
@@ -978,24 +956,24 @@
         <v>-10000000000</v>
       </c>
       <c r="I16" t="str">
-        <v>-10</v>
+        <v>248.49</v>
       </c>
       <c r="J16" t="str">
-        <v>0</v>
+        <v>3154</v>
       </c>
       <c r="K16" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="str">
-        <v>0</v>
+        <v>241.82</v>
       </c>
       <c r="M16" t="str">
-        <v>0</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
-        <v>XBUJ15</v>
+        <v>XBUM15_U15</v>
       </c>
       <c r="C17" t="str">
         <v>XBU</v>
@@ -1004,10 +982,10 @@
         <v>Open</v>
       </c>
       <c r="E17" t="str">
-        <v>FXXXS</v>
+        <v>FMXXS</v>
       </c>
       <c r="F17" t="str">
-        <v>2015-04-24T12:00:00.000Z</v>
+        <v>2015-06-26T12:00:00.000Z</v>
       </c>
       <c r="G17" t="str">
         <v>0.01</v>
@@ -1016,24 +994,24 @@
         <v>-10000000000</v>
       </c>
       <c r="I17" t="str">
-        <v>241.8</v>
+        <v>-10</v>
       </c>
       <c r="J17" t="str">
-        <v>643</v>
+        <v>0</v>
       </c>
       <c r="K17" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" t="str">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="M17" t="str">
-        <v>191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
-        <v>XBU24H</v>
+        <v>XBUJ15</v>
       </c>
       <c r="C18" t="str">
         <v>XBU</v>
@@ -1042,42 +1020,80 @@
         <v>Open</v>
       </c>
       <c r="E18" t="str">
-        <v>FFCCSX</v>
+        <v>FXXXS</v>
       </c>
       <c r="F18" t="str">
-        <v>2015-04-10T12:00:00.000Z</v>
+        <v>2015-04-24T12:00:00.000Z</v>
       </c>
       <c r="G18" t="str">
         <v>0.01</v>
       </c>
       <c r="H18" t="str">
+        <v>-10000000000</v>
+      </c>
+      <c r="I18" t="str">
+        <v>241.8</v>
+      </c>
+      <c r="J18" t="str">
+        <v>644</v>
+      </c>
+      <c r="K18" t="str">
+        <v>2</v>
+      </c>
+      <c r="L18" t="str">
+        <v>240.3792</v>
+      </c>
+      <c r="M18" t="str">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <v>XBU24H</v>
+      </c>
+      <c r="C19" t="str">
+        <v>XBU</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Open</v>
+      </c>
+      <c r="E19" t="str">
+        <v>FFCCSX</v>
+      </c>
+      <c r="F19" t="str">
+        <v>2015-04-10T12:00:00.000Z</v>
+      </c>
+      <c r="G19" t="str">
+        <v>0.01</v>
+      </c>
+      <c r="H19" t="str">
         <v>-100000000</v>
       </c>
-      <c r="I18" t="str">
+      <c r="I19" t="str">
         <v>244.38</v>
       </c>
-      <c r="J18" t="str">
+      <c r="J19" t="str">
         <v>338580</v>
       </c>
-      <c r="K18" t="str">
+      <c r="K19" t="str">
         <v>250</v>
       </c>
-      <c r="L18" t="str">
+      <c r="L19" t="str">
         <v>242.0001</v>
       </c>
-      <c r="M18" t="str">
+      <c r="M19" t="str">
         <v>500</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:M37">
+  <conditionalFormatting sqref="B13:M38">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>VALUE($K12)&gt;0</formula>
+      <formula>VALUE($K13)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>$B$12:$B$18</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
+      <formula1>$B$13:$B$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Additional fields on instruments.
</commit_message>
<xml_diff>
--- a/BitMexExample.xlsx
+++ b/BitMexExample.xlsx
@@ -38,9 +38,6 @@
     <t>AskVol</t>
   </si>
   <si>
-    <t>select product -&gt;</t>
-  </si>
-  <si>
     <t>display depth -&gt;</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>TotAskVol</t>
+  </si>
+  <si>
+    <t>select product from dropdown -&gt;</t>
   </si>
 </sst>
 </file>
@@ -201,9 +201,41 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.317eb5f624984b53bca19561ccc7fb18">
-      <tp>
-        <v>242</v>
+    <main first="rtdsrv.14d02e8123d44e01a20e5a521db4e2e6">
+      <tp>
+        <v>244.56</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Ask</stp>
+        <stp>4</stp>
+        <tr r="F12" s="1"/>
+      </tp>
+      <tp>
+        <v>240.15</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Ask</stp>
+        <stp>3</stp>
+        <tr r="F11" s="1"/>
+      </tp>
+      <tp>
+        <v>240.06</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Ask</stp>
+        <stp>2</stp>
+        <tr r="F10" s="1"/>
+      </tp>
+      <tp>
+        <v>239.7</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Ask</stp>
+        <stp>1</stp>
+        <tr r="F9" s="1"/>
+      </tp>
+      <tp>
+        <v>239.34</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Ask</stp>
@@ -211,79 +243,97 @@
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>242.79</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Ask</stp>
+        <v>231.26</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Bid</stp>
+        <stp>4</stp>
+        <tr r="E12" s="1"/>
+      </tp>
+      <tp>
+        <v>238.27</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Bid</stp>
+        <stp>0</stp>
+        <tr r="E8" s="1"/>
+      </tp>
+      <tp>
+        <v>237.92</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Bid</stp>
         <stp>1</stp>
-        <tr r="F9" s="1"/>
-      </tp>
-      <tp>
-        <v>244</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Ask</stp>
+        <tr r="E9" s="1"/>
+      </tp>
+      <tp>
+        <v>237.7</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>Bid</stp>
         <stp>2</stp>
-        <tr r="F10" s="1"/>
-      </tp>
-      <tp>
-        <v>244.1</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Ask</stp>
-        <stp>3</stp>
-        <tr r="F11" s="1"/>
-      </tp>
-      <tp>
-        <v>246</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Ask</stp>
-        <stp>4</stp>
-        <tr r="F12" s="1"/>
-      </tp>
-      <tp>
-        <v>234.01</v>
+        <tr r="E10" s="1"/>
+      </tp>
+      <tp>
+        <v>237.56</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>Bid</stp>
         <stp>3</stp>
         <tr r="E11" s="1"/>
       </tp>
-      <tp>
-        <v>236</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Bid</stp>
+    </main>
+    <main first="rtdsrv.14d02e8123d44e01a20e5a521db4e2e6">
+      <tp>
+        <v>300</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
+        <stp>4</stp>
+        <tr r="D12" s="1"/>
+      </tp>
+      <tp>
+        <v>1000</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
+        <stp>1</stp>
+        <tr r="D9" s="1"/>
+      </tp>
+      <tp>
+        <v>1000</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
+        <stp>0</stp>
+        <tr r="D8" s="1"/>
+      </tp>
+      <tp>
+        <v>1000</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
+        <stp>3</stp>
+        <tr r="D11" s="1"/>
+      </tp>
+      <tp>
+        <v>400</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>BidVol</stp>
         <stp>2</stp>
-        <tr r="E10" s="1"/>
-      </tp>
-      <tp>
-        <v>238</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Bid</stp>
-        <stp>1</stp>
-        <tr r="E9" s="1"/>
-      </tp>
-      <tp>
-        <v>240</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Bid</stp>
-        <stp>0</stp>
-        <tr r="E8" s="1"/>
-      </tp>
-      <tp>
-        <v>234</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>Bid</stp>
+        <tr r="D10" s="1"/>
+      </tp>
+      <tp>
+        <v>818</v>
+        <stp/>
+        <stp>XBTJ15</stp>
+        <stp>AskVol</stp>
         <stp>4</stp>
-        <tr r="E12" s="1"/>
-      </tp>
-      <tp>
-        <v>300</v>
+        <tr r="G12" s="1"/>
+      </tp>
+      <tp>
+        <v>1000</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
@@ -291,7 +341,7 @@
         <tr r="G9" s="1"/>
       </tp>
       <tp>
-        <v>500</v>
+        <v>1000</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
@@ -299,7 +349,7 @@
         <tr r="G8" s="1"/>
       </tp>
       <tp>
-        <v>819</v>
+        <v>400</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
@@ -307,60 +357,12 @@
         <tr r="G11" s="1"/>
       </tp>
       <tp>
-        <v>500</v>
+        <v>1000</v>
         <stp/>
         <stp>XBTJ15</stp>
         <stp>AskVol</stp>
         <stp>2</stp>
         <tr r="G10" s="1"/>
-      </tp>
-      <tp>
-        <v>500</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>4</stp>
-        <tr r="G12" s="1"/>
-      </tp>
-      <tp>
-        <v>500</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>1</stp>
-        <tr r="D9" s="1"/>
-      </tp>
-      <tp>
-        <v>500</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>0</stp>
-        <tr r="D8" s="1"/>
-      </tp>
-      <tp>
-        <v>300</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>3</stp>
-        <tr r="D11" s="1"/>
-      </tp>
-      <tp>
-        <v>500</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>2</stp>
-        <tr r="D10" s="1"/>
-      </tp>
-      <tp>
-        <v>500</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>4</stp>
-        <tr r="D12" s="1"/>
       </tp>
     </main>
   </volType>
@@ -630,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M22"/>
+  <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,47 +650,49 @@
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(B2, $B$15:$M$22, 7, FALSE)</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(B2, $B$15:$M$22, 2, FALSE)</f>
         <v>XBT</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="str">
         <f>LEFT(VLOOKUP(B2, $B$15:$M$22, 5, FALSE), 10)</f>
         <v>2015-04-24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>2</v>
@@ -703,178 +707,178 @@
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="6">
         <f>D8</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D8" s="3">
         <f>_xll.BitMexBidVol($B$2, $B8)</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="3">
         <f>_xll.BitMexBid($B$2, $B8)</f>
-        <v>240</v>
+        <v>238.27</v>
       </c>
       <c r="F8" s="4">
         <f>_xll.BitMexAsk($B$2, $B8)</f>
-        <v>242</v>
+        <v>239.34</v>
       </c>
       <c r="G8" s="4">
         <f>_xll.BitMexAskVol($B$2, $B8)</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H8" s="6">
         <f>G8</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="6">
         <f>C8+D9</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D9" s="3">
         <f>_xll.BitMexBidVol($B$2, $B9)</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="E9" s="3">
         <f>_xll.BitMexBid($B$2, $B9)</f>
-        <v>238</v>
+        <v>237.92</v>
       </c>
       <c r="F9" s="4">
         <f>_xll.BitMexAsk($B$2, $B9)</f>
-        <v>242.79</v>
+        <v>239.7</v>
       </c>
       <c r="G9" s="4">
         <f>_xll.BitMexAskVol($B$2, $B9)</f>
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="H9" s="6">
         <f>G9+H8</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" ref="C10:C12" si="0">C9+D10</f>
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="D10" s="3">
         <f>_xll.BitMexBidVol($B$2, $B10)</f>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="E10" s="3">
         <f>_xll.BitMexBid($B$2, $B10)</f>
-        <v>236</v>
+        <v>237.7</v>
       </c>
       <c r="F10" s="4">
         <f>_xll.BitMexAsk($B$2, $B10)</f>
-        <v>244</v>
+        <v>240.06</v>
       </c>
       <c r="G10" s="4">
         <f>_xll.BitMexAskVol($B$2, $B10)</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" ref="H10:H12" si="1">G10+H9</f>
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>3400</v>
       </c>
       <c r="D11" s="3">
         <f>_xll.BitMexBidVol($B$2, $B11)</f>
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="3">
         <f>_xll.BitMexBid($B$2, $B11)</f>
-        <v>234.01</v>
+        <v>237.56</v>
       </c>
       <c r="F11" s="4">
         <f>_xll.BitMexAsk($B$2, $B11)</f>
-        <v>244.1</v>
+        <v>240.15</v>
       </c>
       <c r="G11" s="4">
         <f>_xll.BitMexAskVol($B$2, $B11)</f>
-        <v>819</v>
+        <v>400</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="1"/>
-        <v>2119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>2300</v>
+        <v>3700</v>
       </c>
       <c r="D12" s="3">
         <f>_xll.BitMexBidVol($B$2, $B12)</f>
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E12" s="3">
         <f>_xll.BitMexBid($B$2, $B12)</f>
-        <v>234</v>
+        <v>231.26</v>
       </c>
       <c r="F12" s="4">
         <f>_xll.BitMexAsk($B$2, $B12)</f>
-        <v>246</v>
+        <v>244.56</v>
       </c>
       <c r="G12" s="4">
         <f>_xll.BitMexAskVol($B$2, $B12)</f>
-        <v>500</v>
+        <v>818</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="1"/>
-        <v>2619</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="5" t="str">
-        <f t="array" ref="B15:M22">_xll.BitMexInstrumentsActive()</f>
+        <f t="array" ref="B15:T22">_xll.BitMexInstrumentsActive()</f>
         <v>Symbol</v>
       </c>
       <c r="C15" s="5" t="str">
@@ -910,10 +914,31 @@
       <c r="M15" s="5" t="str">
         <v>OpenInterest</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="str">
+        <v>UnderlyingSymbol</v>
+      </c>
+      <c r="O15" s="5" t="str">
+        <v>SettleCurrency</v>
+      </c>
+      <c r="P15" s="5" t="str">
+        <v>UnderlyingToSettleMultiplier</v>
+      </c>
+      <c r="Q15" s="5" t="str">
+        <v>IsQuanto</v>
+      </c>
+      <c r="R15" s="5" t="str">
+        <v>IsInverse</v>
+      </c>
+      <c r="S15" s="5" t="str">
+        <v>High</v>
+      </c>
+      <c r="T15" s="5" t="str">
+        <v>Low</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="str">
         <v>BVOLJ15</v>
@@ -951,8 +976,29 @@
       <c r="M16" t="str">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="str">
+        <v>.BVOL</v>
+      </c>
+      <c r="O16" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P16" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>True</v>
+      </c>
+      <c r="R16" t="str">
+        <v>False</v>
+      </c>
+      <c r="S16" t="str">
+        <v>0</v>
+      </c>
+      <c r="T16" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <v>XBTJ15</v>
       </c>
@@ -989,8 +1035,29 @@
       <c r="M17" t="str">
         <v>54968</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O17" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P17" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>True</v>
+      </c>
+      <c r="R17" t="str">
+        <v>False</v>
+      </c>
+      <c r="S17" t="str">
+        <v>0</v>
+      </c>
+      <c r="T17" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <v>XBUU15</v>
       </c>
@@ -1027,8 +1094,29 @@
       <c r="M18" t="str">
         <v>2211</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O18" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P18" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>False</v>
+      </c>
+      <c r="R18" t="str">
+        <v>True</v>
+      </c>
+      <c r="S18" t="str">
+        <v>0</v>
+      </c>
+      <c r="T18" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <v>XBUM15</v>
       </c>
@@ -1051,22 +1139,43 @@
         <v>-10000000000</v>
       </c>
       <c r="I19" t="str">
-        <v>238.5</v>
+        <v>238</v>
       </c>
       <c r="J19" t="str">
         <v>3267</v>
       </c>
       <c r="K19" t="str">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L19" t="str">
-        <v>238</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
         <v>1095</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O19" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P19" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>False</v>
+      </c>
+      <c r="R19" t="str">
+        <v>True</v>
+      </c>
+      <c r="S19" t="str">
+        <v>0</v>
+      </c>
+      <c r="T19" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <v>XBUM15_U15</v>
       </c>
@@ -1103,8 +1212,29 @@
       <c r="M20" t="str">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N20" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O20" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P20" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>False</v>
+      </c>
+      <c r="R20" t="str">
+        <v>True</v>
+      </c>
+      <c r="S20" t="str">
+        <v>0</v>
+      </c>
+      <c r="T20" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <v>XBUJ15</v>
       </c>
@@ -1127,22 +1257,43 @@
         <v>-10000000000</v>
       </c>
       <c r="I21" t="str">
-        <v>237.99</v>
+        <v>236</v>
       </c>
       <c r="J21" t="str">
         <v>816</v>
       </c>
       <c r="K21" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L21" t="str">
-        <v>236</v>
+        <v>0</v>
       </c>
       <c r="M21" t="str">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N21" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O21" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P21" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>False</v>
+      </c>
+      <c r="R21" t="str">
+        <v>True</v>
+      </c>
+      <c r="S21" t="str">
+        <v>0</v>
+      </c>
+      <c r="T21" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <v>XBU24H</v>
       </c>
@@ -1156,7 +1307,7 @@
         <v>FFCCSX</v>
       </c>
       <c r="F22" t="str">
-        <v>2015-04-11T12:00:00.000Z</v>
+        <v>2015-04-12T12:00:00.000Z</v>
       </c>
       <c r="G22" t="str">
         <v>0.01</v>
@@ -1165,23 +1316,44 @@
         <v>-100000000</v>
       </c>
       <c r="I22" t="str">
-        <v>237.63</v>
+        <v>235.08</v>
       </c>
       <c r="J22" t="str">
-        <v>343234</v>
+        <v>343338</v>
       </c>
       <c r="K22" t="str">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L22" t="str">
-        <v>235</v>
+        <v>0</v>
       </c>
       <c r="M22" t="str">
-        <v>104</v>
+        <v>0</v>
+      </c>
+      <c r="N22" t="str">
+        <v>XBT=</v>
+      </c>
+      <c r="O22" t="str">
+        <v>XBt</v>
+      </c>
+      <c r="P22" t="str">
+        <v>100000000</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>False</v>
+      </c>
+      <c r="R22" t="str">
+        <v>True</v>
+      </c>
+      <c r="S22" t="str">
+        <v>0</v>
+      </c>
+      <c r="T22" t="str">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B16:M41">
+  <conditionalFormatting sqref="B16:T41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>VALUE($K16)&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add =BitMexLastPrice(). Requires additional instrument data and trade subscription
</commit_message>
<xml_diff>
--- a/BitMexExample.xlsx
+++ b/BitMexExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Bid</t>
   </si>
@@ -44,9 +44,6 @@
     <t>instrument download -&gt;</t>
   </si>
   <si>
-    <t>XBTJ15</t>
-  </si>
-  <si>
     <t>(automatically updates)</t>
   </si>
   <si>
@@ -72,6 +69,12 @@
   </si>
   <si>
     <t>select product from dropdown -&gt;</t>
+  </si>
+  <si>
+    <t>Last Price</t>
+  </si>
+  <si>
+    <t>XBU24H</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -172,6 +175,8 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -201,168 +206,177 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.14d02e8123d44e01a20e5a521db4e2e6">
-      <tp>
-        <v>244.56</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+    <main first="rtdsrv.2c889964a5f94d7ab8f475c7c998a5bc">
+      <tp>
+        <v>235.96</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>Last</stp>
+        <tr r="K7" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.2c889964a5f94d7ab8f475c7c998a5bc">
+      <tp>
+        <v>240.11</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Ask</stp>
         <stp>4</stp>
         <tr r="F12" s="1"/>
       </tp>
       <tp>
-        <v>240.15</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>238.88</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Ask</stp>
         <stp>3</stp>
         <tr r="F11" s="1"/>
       </tp>
       <tp>
-        <v>240.06</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>237.89</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Ask</stp>
         <stp>2</stp>
         <tr r="F10" s="1"/>
       </tp>
       <tp>
-        <v>239.7</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>237.54</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Ask</stp>
         <stp>1</stp>
         <tr r="F9" s="1"/>
       </tp>
       <tp>
-        <v>239.34</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>237.18</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Ask</stp>
         <stp>0</stp>
         <tr r="F8" s="1"/>
       </tp>
       <tp>
-        <v>231.26</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>235.34</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Bid</stp>
         <stp>4</stp>
         <tr r="E12" s="1"/>
       </tp>
       <tp>
-        <v>238.27</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>236.05</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Bid</stp>
         <stp>0</stp>
         <tr r="E8" s="1"/>
       </tp>
       <tp>
-        <v>237.92</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>235.79</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Bid</stp>
         <stp>1</stp>
         <tr r="E9" s="1"/>
       </tp>
       <tp>
-        <v>237.7</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>235.78</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Bid</stp>
         <stp>2</stp>
         <tr r="E10" s="1"/>
       </tp>
       <tp>
-        <v>237.56</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <v>235.69</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>Bid</stp>
         <stp>3</stp>
         <tr r="E11" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.14d02e8123d44e01a20e5a521db4e2e6">
-      <tp>
-        <v>300</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>BidVol</stp>
+        <stp>0</stp>
+        <tr r="D8" s="1"/>
+      </tp>
+      <tp>
+        <v>100</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>BidVol</stp>
+        <stp>1</stp>
+        <tr r="D9" s="1"/>
+      </tp>
+      <tp>
+        <v>1000</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>BidVol</stp>
+        <stp>2</stp>
+        <tr r="D10" s="1"/>
+      </tp>
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>BidVol</stp>
+        <stp>3</stp>
+        <tr r="D11" s="1"/>
+      </tp>
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
         <stp>BidVol</stp>
         <stp>4</stp>
         <tr r="D12" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.2c889964a5f94d7ab8f475c7c998a5bc">
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>AskVol</stp>
+        <stp>0</stp>
+        <tr r="G8" s="1"/>
+      </tp>
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>AskVol</stp>
+        <stp>1</stp>
+        <tr r="G9" s="1"/>
+      </tp>
+      <tp>
+        <v>500</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>AskVol</stp>
+        <stp>2</stp>
+        <tr r="G10" s="1"/>
+      </tp>
+      <tp>
+        <v>100</v>
+        <stp/>
+        <stp>XBU24H</stp>
+        <stp>AskVol</stp>
+        <stp>3</stp>
+        <tr r="G11" s="1"/>
+      </tp>
       <tp>
         <v>1000</v>
         <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>1</stp>
-        <tr r="D9" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>0</stp>
-        <tr r="D8" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>3</stp>
-        <tr r="D11" s="1"/>
-      </tp>
-      <tp>
-        <v>400</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>BidVol</stp>
-        <stp>2</stp>
-        <tr r="D10" s="1"/>
-      </tp>
-      <tp>
-        <v>818</v>
-        <stp/>
-        <stp>XBTJ15</stp>
+        <stp>XBU24H</stp>
         <stp>AskVol</stp>
         <stp>4</stp>
         <tr r="G12" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>1</stp>
-        <tr r="G9" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>0</stp>
-        <tr r="G8" s="1"/>
-      </tp>
-      <tp>
-        <v>400</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>3</stp>
-        <tr r="G11" s="1"/>
-      </tp>
-      <tp>
-        <v>1000</v>
-        <stp/>
-        <stp>XBTJ15</stp>
-        <stp>AskVol</stp>
-        <stp>2</stp>
-        <tr r="G10" s="1"/>
       </tp>
     </main>
   </volType>
@@ -635,7 +649,7 @@
   <dimension ref="A2:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,43 +670,46 @@
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="str">
         <f>VLOOKUP(B2, $B$15:$M$22, 7, FALSE)</f>
-        <v>1000</v>
+        <v>-100000000</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="str">
         <f>VLOOKUP(B2, $B$15:$M$22, 2, FALSE)</f>
-        <v>XBT</v>
+        <v>XBU</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="str">
         <f>LEFT(VLOOKUP(B2, $B$15:$M$22, 5, FALSE), 10)</f>
-        <v>2015-04-24</v>
+        <v>2015-04-12</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>2</v>
@@ -707,71 +724,78 @@
         <v>3</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1">
+        <f>_xll.BitMexLastPrice(B2)</f>
+        <v>235.96</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" s="6">
         <f>D8</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="D8" s="3">
         <f>_xll.BitMexBidVol($B$2, $B8)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E8" s="3">
         <f>_xll.BitMexBid($B$2, $B8)</f>
-        <v>238.27</v>
+        <v>236.05</v>
       </c>
       <c r="F8" s="4">
         <f>_xll.BitMexAsk($B$2, $B8)</f>
-        <v>239.34</v>
+        <v>237.18</v>
       </c>
       <c r="G8" s="4">
         <f>_xll.BitMexAskVol($B$2, $B8)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H8" s="6">
         <f>G8</f>
-        <v>1000</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="7"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="6">
         <f>C8+D9</f>
-        <v>2000</v>
+        <v>600</v>
       </c>
       <c r="D9" s="3">
         <f>_xll.BitMexBidVol($B$2, $B9)</f>
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="E9" s="3">
         <f>_xll.BitMexBid($B$2, $B9)</f>
-        <v>237.92</v>
+        <v>235.79</v>
       </c>
       <c r="F9" s="4">
         <f>_xll.BitMexAsk($B$2, $B9)</f>
-        <v>239.7</v>
+        <v>237.54</v>
       </c>
       <c r="G9" s="4">
         <f>_xll.BitMexAskVol($B$2, $B9)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H9" s="6">
         <f>G9+H8</f>
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -780,27 +804,27 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ref="C10:C12" si="0">C9+D10</f>
-        <v>2400</v>
+        <v>1600</v>
       </c>
       <c r="D10" s="3">
         <f>_xll.BitMexBidVol($B$2, $B10)</f>
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="E10" s="3">
         <f>_xll.BitMexBid($B$2, $B10)</f>
-        <v>237.7</v>
+        <v>235.78</v>
       </c>
       <c r="F10" s="4">
         <f>_xll.BitMexAsk($B$2, $B10)</f>
-        <v>240.06</v>
+        <v>237.89</v>
       </c>
       <c r="G10" s="4">
         <f>_xll.BitMexAskVol($B$2, $B10)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" ref="H10:H12" si="1">G10+H9</f>
-        <v>3000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -809,27 +833,27 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
-        <v>3400</v>
+        <v>2100</v>
       </c>
       <c r="D11" s="3">
         <f>_xll.BitMexBidVol($B$2, $B11)</f>
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="E11" s="3">
         <f>_xll.BitMexBid($B$2, $B11)</f>
-        <v>237.56</v>
+        <v>235.69</v>
       </c>
       <c r="F11" s="4">
         <f>_xll.BitMexAsk($B$2, $B11)</f>
-        <v>240.15</v>
+        <v>238.88</v>
       </c>
       <c r="G11" s="4">
         <f>_xll.BitMexAskVol($B$2, $B11)</f>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" si="1"/>
-        <v>3400</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -838,27 +862,27 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" si="0"/>
-        <v>3700</v>
+        <v>2600</v>
       </c>
       <c r="D12" s="3">
         <f>_xll.BitMexBidVol($B$2, $B12)</f>
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="E12" s="3">
         <f>_xll.BitMexBid($B$2, $B12)</f>
-        <v>231.26</v>
+        <v>235.34</v>
       </c>
       <c r="F12" s="4">
         <f>_xll.BitMexAsk($B$2, $B12)</f>
-        <v>244.56</v>
+        <v>240.11</v>
       </c>
       <c r="G12" s="4">
         <f>_xll.BitMexAskVol($B$2, $B12)</f>
-        <v>818</v>
+        <v>1000</v>
       </c>
       <c r="H12" s="6">
         <f t="shared" si="1"/>
-        <v>4218</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -938,7 +962,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="str">
         <v>BVOLJ15</v>
@@ -965,16 +989,16 @@
         <v>60</v>
       </c>
       <c r="J16" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K16" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L16" t="str">
-        <v>0</v>
+        <v>61.76</v>
       </c>
       <c r="M16" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" t="str">
         <v>.BVOL</v>
@@ -992,10 +1016,10 @@
         <v>False</v>
       </c>
       <c r="S16" t="str">
-        <v>0</v>
+        <v>63.52</v>
       </c>
       <c r="T16" t="str">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
@@ -1024,13 +1048,13 @@
         <v>241</v>
       </c>
       <c r="J17" t="str">
-        <v>204890</v>
+        <v>205645</v>
       </c>
       <c r="K17" t="str">
-        <v>0</v>
+        <v>755</v>
       </c>
       <c r="L17" t="str">
-        <v>0</v>
+        <v>240.971</v>
       </c>
       <c r="M17" t="str">
         <v>54968</v>
@@ -1051,10 +1075,10 @@
         <v>False</v>
       </c>
       <c r="S17" t="str">
-        <v>0</v>
+        <v>242.62</v>
       </c>
       <c r="T17" t="str">
-        <v>0</v>
+        <v>239.68</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
@@ -1319,16 +1343,16 @@
         <v>235.08</v>
       </c>
       <c r="J22" t="str">
-        <v>343338</v>
+        <v>343438</v>
       </c>
       <c r="K22" t="str">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L22" t="str">
-        <v>0</v>
+        <v>235.9598</v>
       </c>
       <c r="M22" t="str">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N22" t="str">
         <v>XBT=</v>
@@ -1346,10 +1370,10 @@
         <v>True</v>
       </c>
       <c r="S22" t="str">
-        <v>0</v>
+        <v>235.96</v>
       </c>
       <c r="T22" t="str">
-        <v>0</v>
+        <v>235.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>